<commit_message>
manuscript draft text and metadata created
</commit_message>
<xml_diff>
--- a/species.xlsx
+++ b/species.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slane84\OneDrive - The University Of British Columbia\Documents\Dissertation\HabitatRecovery\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/stefanie_lane_ubc_ca/Documents/Documents/Dissertation/HabitatRecovery/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A4FE87-1251-466A-A627-AE1AF1F27477}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{66CF8C71-F571-4A69-920A-D783860CAA27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{BBB8E670-FD30-408F-B694-695B488B79B0}"/>
   </bookViews>
@@ -250,12 +250,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -270,8 +276,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,7 +596,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A19" sqref="A19:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1015,10 +1022,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C19" t="s">
@@ -1208,6 +1215,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100483727557648AA40B029C215891F95C5" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d36f379eec1cf084072dcf956aecbcf8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8c008993-a31f-4b40-b1f3-88dd9c6e1924" xmlns:ns4="360018dd-41eb-4458-b1d4-4b46a95a2b02" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd1f472f1ef3281fe4dbeb8213942d38" ns3:_="" ns4:_="">
     <xsd:import namespace="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
@@ -1436,12 +1449,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1452,6 +1459,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C816B061-1CDD-439F-8C9F-29C9EF4FB231}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="360018dd-41eb-4458-b1d4-4b46a95a2b02"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34E72DEF-7AF1-4F07-B46B-983AB5556665}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1470,23 +1494,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C816B061-1CDD-439F-8C9F-29C9EF4FB231}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="360018dd-41eb-4458-b1d4-4b46a95a2b02"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CBD582-CD76-4265-9BA2-35ECC89DA4D4}">
   <ds:schemaRefs>

</xml_diff>